<commit_message>
Removed Acquisition date from Adult Learning Project metadata
</commit_message>
<xml_diff>
--- a/Photographic Archive/ADULT LEARNING PROJECT COLLECTION.xlsx
+++ b/Photographic Archive/ADULT LEARNING PROJECT COLLECTION.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="178">
   <si>
     <t>identifier</t>
   </si>
@@ -46,21 +46,6 @@
     <t>Item</t>
   </si>
   <si>
-    <t>ITEM DESCRIPTION</t>
-  </si>
-  <si>
-    <t>LOCATION | SECTION</t>
-  </si>
-  <si>
-    <t>ACCESSION NO</t>
-  </si>
-  <si>
-    <t>TITLE</t>
-  </si>
-  <si>
-    <t>ACQUISITION NO.</t>
-  </si>
-  <si>
     <t>QTY</t>
   </si>
   <si>
@@ -77,9 +62,6 @@
   </si>
   <si>
     <t>MARY BENSON</t>
-  </si>
-  <si>
-    <t>01/04/2014</t>
   </si>
   <si>
     <t>RC-B/W  PRINT</t>
@@ -851,11 +833,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z67"/>
+  <dimension ref="A1:Z66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -864,9 +846,10 @@
     <col min="3" max="3" width="47" customWidth="1"/>
     <col min="5" max="5" width="15.109375" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" customWidth="1"/>
-    <col min="8" max="9" width="92.33203125" customWidth="1"/>
-    <col min="11" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="11" max="14" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -896,10 +879,18 @@
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -915,1522 +906,1418 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="D2" s="5"/>
       <c r="E2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="K2" t="s">
-        <v>14</v>
+        <v>16</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D3" s="5"/>
       <c r="E3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G3" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
         <v>22</v>
       </c>
-      <c r="K3">
-        <v>1</v>
-      </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>23</v>
       </c>
-      <c r="M3" t="s">
-        <v>24</v>
-      </c>
       <c r="N3" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4" t="s">
         <v>27</v>
       </c>
-      <c r="D4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M4" t="s">
-        <v>29</v>
-      </c>
       <c r="N4" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
+      <c r="L5" t="s">
         <v>30</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K5">
-        <v>1</v>
-      </c>
-      <c r="L5" t="s">
-        <v>33</v>
-      </c>
       <c r="N5" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D6" s="5"/>
       <c r="E6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="N6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7">
+        <v>1</v>
+      </c>
+      <c r="L7" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7" t="s">
-        <v>39</v>
-      </c>
       <c r="N7" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8">
-        <v>1</v>
-      </c>
-      <c r="L8" t="s">
-        <v>43</v>
-      </c>
       <c r="N8" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D9" s="5"/>
       <c r="E9" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K9">
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="N9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10">
+        <v>1</v>
+      </c>
+      <c r="L10" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10" t="s">
-        <v>49</v>
-      </c>
       <c r="N10" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K11">
+        <v>1</v>
+      </c>
+      <c r="L11" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-      <c r="L11" t="s">
-        <v>53</v>
-      </c>
       <c r="N11" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D12" s="5"/>
       <c r="E12" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K12">
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="N12" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D13" s="5"/>
       <c r="E13" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="N13" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D14" s="5"/>
       <c r="E14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K14">
         <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="N14" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="5"/>
+      <c r="E15" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K15">
+        <v>1</v>
+      </c>
+      <c r="L15" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15">
-        <v>1</v>
-      </c>
-      <c r="L15" t="s">
-        <v>63</v>
-      </c>
       <c r="N15" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D16" s="5"/>
       <c r="E16" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K16">
         <v>1</v>
       </c>
       <c r="L16" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="N16" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K17">
         <v>1</v>
       </c>
       <c r="L17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="N17" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="5"/>
+      <c r="E18" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K18">
+        <v>1</v>
+      </c>
+      <c r="L18" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G18" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18">
-        <v>1</v>
-      </c>
-      <c r="L18" t="s">
-        <v>71</v>
-      </c>
       <c r="N18" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K19">
         <v>1</v>
       </c>
       <c r="L19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="N19" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D20" s="5"/>
       <c r="E20" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K20">
         <v>1</v>
       </c>
       <c r="L20" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="N20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D21" s="5"/>
       <c r="E21" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K21">
         <v>1</v>
       </c>
       <c r="L21" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="N21" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="D22" s="5"/>
       <c r="E22" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K22">
         <v>1</v>
       </c>
       <c r="L22" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="N22" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D23" s="5"/>
       <c r="E23" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K23">
         <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="N23" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>83</v>
+      </c>
+      <c r="D24" s="5"/>
       <c r="E24" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K24">
         <v>1</v>
       </c>
       <c r="L24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="N24" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25" t="s">
+        <v>87</v>
+      </c>
+      <c r="N25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-      <c r="L25" t="s">
+      <c r="D26" s="5"/>
+      <c r="E26" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26" t="s">
         <v>90</v>
       </c>
-      <c r="N25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26">
-        <v>1</v>
-      </c>
-      <c r="L26" t="s">
-        <v>93</v>
-      </c>
       <c r="N26" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="D27" s="5"/>
       <c r="E27" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="K27">
         <v>1</v>
       </c>
       <c r="L27" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="N27" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D28" s="5"/>
       <c r="E28" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>32</v>
+        <v>95</v>
       </c>
       <c r="K28">
         <v>1</v>
       </c>
       <c r="L28" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="N28" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="D29" s="5"/>
       <c r="E29" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K29">
         <v>1</v>
       </c>
       <c r="L29" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="N29" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D30" s="5"/>
       <c r="E30" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K30">
         <v>1</v>
       </c>
       <c r="L30" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="N30" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D31" s="5"/>
       <c r="E31" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K31">
         <v>1</v>
       </c>
       <c r="L31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="N31" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="32" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D32" s="5"/>
+      <c r="E32" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K32">
+        <v>1</v>
+      </c>
+      <c r="L32" t="s">
+        <v>106</v>
+      </c>
+      <c r="N32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K33">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G32" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K32">
-        <v>1</v>
-      </c>
-      <c r="L32" t="s">
+      <c r="N33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="N32" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="C34" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D33" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E33" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G33" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K33">
-        <v>1</v>
-      </c>
-      <c r="L33" t="s">
+      <c r="D34" s="5"/>
+      <c r="E34" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="K34">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
         <v>112</v>
       </c>
-      <c r="N33" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E34" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K34">
-        <v>1</v>
-      </c>
-      <c r="L34" t="s">
-        <v>115</v>
-      </c>
       <c r="N34" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D35" s="5"/>
       <c r="E35" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K35">
         <v>1</v>
       </c>
       <c r="L35" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="N35" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="36" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>117</v>
+      </c>
+      <c r="D36" s="5"/>
       <c r="E36" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K36">
         <v>1</v>
       </c>
       <c r="L36" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="N36" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D37" s="5"/>
       <c r="E37" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K37">
         <v>1</v>
       </c>
       <c r="L37" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="N37" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="38" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="D38" s="5"/>
       <c r="E38" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K38">
         <v>1</v>
       </c>
       <c r="L38" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="N38" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="D39" s="5"/>
       <c r="E39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K39">
         <v>1</v>
       </c>
       <c r="L39" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="N39" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="D40" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D40" s="5"/>
       <c r="E40" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K40">
         <v>1</v>
       </c>
       <c r="L40" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="N40" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="D41" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>130</v>
+      </c>
+      <c r="D41" s="5"/>
       <c r="E41" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K41">
         <v>1</v>
       </c>
       <c r="L41" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="N41" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D42" s="5"/>
       <c r="E42" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F42" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K42">
         <v>1</v>
       </c>
       <c r="L42" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="N42" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="43" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>101</v>
+      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K43">
         <v>1</v>
       </c>
       <c r="L43" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="N43" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="D44" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="D44" s="5"/>
       <c r="E44" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K44">
         <v>1</v>
       </c>
       <c r="L44" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="N44" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="45" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D45" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>139</v>
+      </c>
+      <c r="D45" s="5"/>
       <c r="E45" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K45">
         <v>1</v>
       </c>
       <c r="L45" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="N45" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D46" s="5"/>
       <c r="E46" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K46">
         <v>1</v>
       </c>
       <c r="L46" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="N46" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="47" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="D47" s="5"/>
       <c r="E47" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="K47">
         <v>1</v>
       </c>
       <c r="L47" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="N47" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="48" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D48" s="5"/>
       <c r="E48" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>101</v>
+        <v>146</v>
       </c>
       <c r="K48">
         <v>1</v>
       </c>
       <c r="L48" t="s">
-        <v>150</v>
+        <v>147</v>
+      </c>
+      <c r="M48" t="s">
+        <v>148</v>
       </c>
       <c r="N48" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="49" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="D49" s="5"/>
+      <c r="E49" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G49" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="K49">
+        <v>1</v>
+      </c>
+      <c r="L49" t="s">
         <v>151</v>
       </c>
-      <c r="C49" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E49" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G49" s="6" t="s">
+      <c r="M49" t="s">
         <v>152</v>
       </c>
-      <c r="K49">
-        <v>1</v>
-      </c>
-      <c r="L49" t="s">
-        <v>153</v>
-      </c>
-      <c r="M49" t="s">
-        <v>154</v>
-      </c>
       <c r="N49" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D50" s="5"/>
+      <c r="E50" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F50" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G50" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50" t="s">
+        <v>154</v>
+      </c>
+      <c r="M50" t="s">
         <v>155</v>
       </c>
-      <c r="C50" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E50" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G50" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="K50">
-        <v>1</v>
-      </c>
-      <c r="L50" t="s">
-        <v>157</v>
-      </c>
-      <c r="M50" t="s">
-        <v>158</v>
-      </c>
       <c r="N50" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D51" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="D51" s="5"/>
       <c r="E51" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="K51">
         <v>1</v>
       </c>
       <c r="L51" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="M51" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="N51" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="D52" s="5"/>
       <c r="E52" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="K52">
         <v>1</v>
       </c>
       <c r="L52" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="M52" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="N52" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="53" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F53" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G53" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E53" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="G53" s="6" t="s">
-        <v>152</v>
       </c>
       <c r="K53">
         <v>1</v>
@@ -2438,11 +2325,8 @@
       <c r="L53" t="s">
         <v>166</v>
       </c>
-      <c r="M53" t="s">
+      <c r="N53" t="s">
         <v>167</v>
-      </c>
-      <c r="N53" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
@@ -2450,119 +2334,92 @@
         <v>168</v>
       </c>
       <c r="C54" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D54" s="5"/>
+      <c r="E54" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F54" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="G54" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="K54">
+        <v>1</v>
+      </c>
+      <c r="L54" t="s">
         <v>169</v>
       </c>
-      <c r="D54" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G54" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="K54">
-        <v>1</v>
-      </c>
-      <c r="L54" t="s">
-        <v>172</v>
-      </c>
       <c r="N54" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>20</v>
-      </c>
+        <v>163</v>
+      </c>
+      <c r="D55" s="5"/>
       <c r="E55" s="6" t="s">
         <v>8</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G55" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="K55">
+        <v>1</v>
+      </c>
+      <c r="L55" t="s">
         <v>171</v>
       </c>
-      <c r="K55">
-        <v>1</v>
-      </c>
-      <c r="L55" t="s">
-        <v>175</v>
-      </c>
       <c r="N55" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="5"/>
+      <c r="E56" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="K56">
+        <v>1</v>
+      </c>
+      <c r="L56" t="s">
         <v>176</v>
       </c>
-      <c r="C56" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E56" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="G56" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="K56">
-        <v>1</v>
-      </c>
-      <c r="L56" t="s">
+      <c r="M56" t="s">
         <v>177</v>
       </c>
       <c r="N56" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="G57" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="K57">
-        <v>1</v>
-      </c>
-      <c r="L57" t="s">
-        <v>182</v>
-      </c>
-      <c r="M57" t="s">
-        <v>183</v>
-      </c>
-      <c r="N57" t="s">
-        <v>173</v>
-      </c>
+      <c r="A57" s="3"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
     </row>
     <row r="58" spans="1:14" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A58" s="3"/>
@@ -2636,14 +2493,6 @@
       <c r="F66" s="6"/>
       <c r="G66" s="6"/>
     </row>
-    <row r="67" spans="1:7" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A67" s="3"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="6"/>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6"/>
-    </row>
   </sheetData>
   <autoFilter ref="A1:Z1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated collections in Adult learning project collection from auditors register
</commit_message>
<xml_diff>
--- a/Photographic Archive/ADULT LEARNING PROJECT COLLECTION.xlsx
+++ b/Photographic Archive/ADULT LEARNING PROJECT COLLECTION.xlsx
@@ -12,7 +12,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -835,9 +835,9 @@
   </sheetPr>
   <dimension ref="A1:Z66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>